<commit_message>
re-enable equity option example in excel
</commit_message>
<xml_diff>
--- a/Workbooks/EquityOption.xlsx
+++ b/Workbooks/EquityOption.xlsx
@@ -91,12 +91,6 @@
     <t>black constant vol ID</t>
   </si>
   <si>
-    <t>blask scholes process ID</t>
-  </si>
-  <si>
-    <t>blask scholes process object</t>
-  </si>
-  <si>
     <t>flatTermStructure</t>
   </si>
   <si>
@@ -146,6 +140,12 @@
   </si>
   <si>
     <t>npv</t>
+  </si>
+  <si>
+    <t>black scholes process ID</t>
+  </si>
+  <si>
+    <t>black scholes process object</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,7 +559,7 @@
       </c>
       <c r="B1" s="1" t="str">
         <f>_xll.qlVersion()</f>
-        <v>1.5</v>
+        <v>1.6.2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="b">
-        <f>_xll.qlSettingsSetEvaluationDate(B4)</f>
+        <f>_xll.qlSettingsSetEvaluationDate(,B4)</f>
         <v>1</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6">
         <v>0.06</v>
@@ -684,8 +684,8 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="str">
-        <f>_xll.qlEuropeanExercise(B17,B14)</f>
-        <v>europeanExercise#0001</v>
+        <f>_xll.qlEuropeanExercise(B6,B17,,,B14)</f>
+        <v>europeanExercise#0000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -705,8 +705,8 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="str">
-        <f>_xll.qlSimpleQuote(B20,B9)</f>
-        <v>underlying#0001</v>
+        <f>_xll.qlSimpleQuote(B6,B20,,,B9)</f>
+        <v>underlying#0000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -726,8 +726,8 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f>_xll.qlFlatForward(B23,B5,B12,B15)</f>
-        <v>flatTermStructure#0001</v>
+        <f>_xll.qlFlatForward(B6,B23,,,B5,B12,B15)</f>
+        <v>flatTermStructure#0000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -739,7 +739,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -747,8 +747,8 @@
         <v>21</v>
       </c>
       <c r="B27" s="3" t="str">
-        <f>_xll.qlFlatForward(B26,B5,B11,B15)</f>
-        <v>flatDividendTS#0001</v>
+        <f>_xll.qlFlatForward(B6,B26,,,B5,B11,B15)</f>
+        <v>flatDividendTS#0000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -760,7 +760,7 @@
         <v>22</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -768,8 +768,8 @@
         <v>6</v>
       </c>
       <c r="B30" s="3" t="str">
-        <f>_xll.qlBlackConstantVol(B29,B5,B3,B13,B15)</f>
-        <v>flatVolTS#0001</v>
+        <f>_xll.qlBlackConstantVol(B6,B29,,,B5,B3,B13,B15)</f>
+        <v>flatVolTS#0000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -778,103 +778,107 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B33" s="3" t="str">
-        <f>_xll.qlBlackScholesMertonProcess(B32,B21,B26,B23,B29)</f>
+        <f>_xll.qlBlackScholesMertonProcess(,B32,,,B21,B27,B24,B30)</f>
         <v>bsmProcess#0000</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="str">
+        <f>_xll.ohRangeRetrieveError(B33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f>_xll.qlPlainVanillaPayoff(B35,B8,B10)</f>
-        <v>payoff#0001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <f>_xll.qlPlainVanillaPayoff(B6,B35,,,B8,B10)</f>
+        <v>payoff#0000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="str">
-        <f>_xll.qlVanillaOption(B38,B36,B18)</f>
-        <v>europeanOption#0001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <f>_xll.qlVanillaOption(,B38,,,B36,B18)</f>
+        <v>europeanOption#0000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="B42" s="3" t="str">
-        <f>_xll.qlAnalyticEuropeanEngine(B41,B33)</f>
+        <f>_xll.qlAnalyticEuropeanEngine(,B41,,,B33)</f>
         <v>engine#0000</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="b">
-        <f>_xll.qlInstrumentSetPricingEngine(B39,B42)</f>
+        <f>_xll.qlInstrumentSetPricingEngine(,B39,B42)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1">
-        <f>_xll.qlInstrumentNPV(B39)</f>
+        <f>_xll.qlInstrumentNPV(B42,B39)</f>
         <v>3.8443077915968398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save workbook when XLL is not loaded
</commit_message>
<xml_diff>
--- a/Workbooks/EquityOption.xlsx
+++ b/Workbooks/EquityOption.xlsx
@@ -557,9 +557,9 @@
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="str">
-        <f>_xll.qlVersion()</f>
-        <v>1.6.2</v>
+      <c r="B1" s="1" t="e">
+        <f ca="1">_xll.qlVersion()</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -594,9 +594,9 @@
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="b">
-        <f>_xll.qlSettingsSetEvaluationDate(,B4)</f>
-        <v>1</v>
+      <c r="B6" s="3" t="e">
+        <f ca="1">_xll.qlSettingsSetEvaluationDate(,B4)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -683,9 +683,9 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="str">
-        <f>_xll.qlEuropeanExercise(B6,B17,,,B14)</f>
-        <v>europeanExercise#0000</v>
+      <c r="B18" s="3" t="e">
+        <f ca="1">_xll.qlEuropeanExercise(B6,B17,,,B14)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -704,9 +704,9 @@
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="5" t="str">
-        <f>_xll.qlSimpleQuote(B6,B20,,,B9)</f>
-        <v>underlying#0000</v>
+      <c r="B21" s="5" t="e">
+        <f ca="1">_xll.qlSimpleQuote(B6,B20,,,B9)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -725,9 +725,9 @@
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3" t="str">
-        <f>_xll.qlFlatForward(B6,B23,,,B5,B12,B15)</f>
-        <v>flatTermStructure#0000</v>
+      <c r="B24" s="3" t="e">
+        <f ca="1">_xll.qlFlatForward(B6,B23,,,B5,B12,B15)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,9 +746,9 @@
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="3" t="str">
-        <f>_xll.qlFlatForward(B6,B26,,,B5,B11,B15)</f>
-        <v>flatDividendTS#0000</v>
+      <c r="B27" s="3" t="e">
+        <f ca="1">_xll.qlFlatForward(B6,B26,,,B5,B11,B15)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -767,9 +767,9 @@
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="3" t="str">
-        <f>_xll.qlBlackConstantVol(B6,B29,,,B5,B3,B13,B15)</f>
-        <v>flatVolTS#0000</v>
+      <c r="B30" s="3" t="e">
+        <f ca="1">_xll.qlBlackConstantVol(B6,B29,,,B5,B3,B13,B15)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -788,13 +788,13 @@
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="3" t="str">
-        <f>_xll.qlBlackScholesMertonProcess(,B32,,,B21,B27,B24,B30)</f>
-        <v>bsmProcess#0000</v>
-      </c>
-      <c r="C33" s="1" t="str">
-        <f>_xll.ohRangeRetrieveError(B33)</f>
-        <v/>
+      <c r="B33" s="3" t="e">
+        <f ca="1">_xll.qlBlackScholesMertonProcess(,B32,,,B21,B27,B24,B30)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C33" s="1" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(B33)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -813,9 +813,9 @@
       <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="3" t="str">
-        <f>_xll.qlPlainVanillaPayoff(B6,B35,,,B8,B10)</f>
-        <v>payoff#0000</v>
+      <c r="B36" s="3" t="e">
+        <f ca="1">_xll.qlPlainVanillaPayoff(B6,B35,,,B8,B10)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -834,9 +834,9 @@
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="3" t="str">
-        <f>_xll.qlVanillaOption(,B38,,,B36,B18)</f>
-        <v>europeanOption#0000</v>
+      <c r="B39" s="3" t="e">
+        <f ca="1">_xll.qlVanillaOption(,B38,,,B36,B18)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -855,9 +855,9 @@
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="3" t="str">
-        <f>_xll.qlAnalyticEuropeanEngine(,B41,,,B33)</f>
-        <v>engine#0000</v>
+      <c r="B42" s="3" t="e">
+        <f ca="1">_xll.qlAnalyticEuropeanEngine(,B41,,,B33)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -868,18 +868,18 @@
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="3" t="b">
-        <f>_xll.qlInstrumentSetPricingEngine(,B39,B42)</f>
-        <v>1</v>
+      <c r="B44" s="3" t="e">
+        <f ca="1">_xll.qlInstrumentSetPricingEngine(,B39,B42)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="1">
-        <f>_xll.qlInstrumentNPV(B42,B39)</f>
-        <v>3.8443077915968398</v>
+      <c r="B46" s="1" t="e">
+        <f ca="1">_xll.qlInstrumentNPV(B42,B39)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>